<commit_message>
upload february census county/ city codes and sources
upload february census county/ city codes and sources
</commit_message>
<xml_diff>
--- a/sources.xlsx
+++ b/sources.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>最新县及县以上行政区划代码（截止2016年7月31日）.csv</t>
   </si>
@@ -47,10 +47,19 @@
     <t>http://www.mca.gov.cn/article/sj/tjbz/a/2017/20170301/2017%E5%B9%B41%E6%9C%88%E5%8E%BF%E4%BB%A5%E4%B8%8A%E8%A1%8C%E6%94%BF%E5%8C%BA%E5%88%92%E4%BB%A3%E7%A0%81.html</t>
   </si>
   <si>
-    <t>county updates 01/2017</t>
-  </si>
-  <si>
     <t>2017年1月中华人民共和国县以上行政区划代码.csv</t>
+  </si>
+  <si>
+    <t>county updates 01/2017(released 2017-03-01)</t>
+  </si>
+  <si>
+    <t>county updates 02/2017(released 2017-03-27)</t>
+  </si>
+  <si>
+    <t>2017年2月中华人民共和国县以上行政区划代码.csv</t>
+  </si>
+  <si>
+    <t>http://www.mca.gov.cn/article/sj/tjbz/a/2017/0327/2017%E5%B9%B42%E6%9C%88%E4%B8%AD%E5%8D%8E%E4%BA%BA%E6%B0%91%E5%85%B1%E5%92%8C%E5%9B%BD%E5%8E%BF%E4%BB%A5%E4%B8%8A%E8%A1%8C%E6%94%BF%E5%8C%BA%E5%88%92%E4%BB%A3%E7%A0%81.html</t>
   </si>
 </sst>
 </file>
@@ -368,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,16 +414,28 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>